<commit_message>
Updated Tutorial 1 Project Level Setup file a bit
Some refinements and modifications for video Part 3 of tutorial 1
</commit_message>
<xml_diff>
--- a/tutorial_projects/tutorial1/cassandra/inputs/domain_model.xlsx
+++ b/tutorial_projects/tutorial1/cassandra/inputs/domain_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aa_git_repos\aa_non_code_repos\cassandra_default_road_model\tutorial_projects\tutorial1\cassandra\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B24447-5546-41D2-B5D7-9EF862CF537B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415F23F1-C4CB-45A7-BD1F-654B7ECB04FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="669" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7425" yWindow="390" windowWidth="37545" windowHeight="19725" tabRatio="669" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="change_log" sheetId="10" state="hidden" r:id="rId1"/>
@@ -6970,10 +6970,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7415,7 +7415,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7515,9 +7515,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M482"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q22" sqref="Q22"/>
+      <selection pane="bottomLeft" activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -22206,7 +22206,7 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -23190,7 +23190,7 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24190,8 +24190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O260"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24311,17 +24311,17 @@
       <c r="E6" s="120" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="191" t="s">
+      <c r="G6" s="192" t="s">
         <v>1853</v>
       </c>
-      <c r="H6" s="191"/>
-      <c r="I6" s="191"/>
-      <c r="J6" s="191"/>
-      <c r="K6" s="191"/>
-      <c r="L6" s="191"/>
-      <c r="M6" s="191"/>
-      <c r="N6" s="191"/>
-      <c r="O6" s="191"/>
+      <c r="H6" s="192"/>
+      <c r="I6" s="192"/>
+      <c r="J6" s="192"/>
+      <c r="K6" s="192"/>
+      <c r="L6" s="192"/>
+      <c r="M6" s="192"/>
+      <c r="N6" s="192"/>
+      <c r="O6" s="192"/>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="120" t="s">
@@ -24339,15 +24339,15 @@
       <c r="E7" s="120" t="b">
         <v>0</v>
       </c>
-      <c r="G7" s="191"/>
-      <c r="H7" s="191"/>
-      <c r="I7" s="191"/>
-      <c r="J7" s="191"/>
-      <c r="K7" s="191"/>
-      <c r="L7" s="191"/>
-      <c r="M7" s="191"/>
-      <c r="N7" s="191"/>
-      <c r="O7" s="191"/>
+      <c r="G7" s="192"/>
+      <c r="H7" s="192"/>
+      <c r="I7" s="192"/>
+      <c r="J7" s="192"/>
+      <c r="K7" s="192"/>
+      <c r="L7" s="192"/>
+      <c r="M7" s="192"/>
+      <c r="N7" s="192"/>
+      <c r="O7" s="192"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="120" t="s">
@@ -28518,7 +28518,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29135,28 +29135,28 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="191" t="s">
+      <c r="B30" s="192" t="s">
         <v>1854</v>
       </c>
-      <c r="C30" s="191"/>
-      <c r="D30" s="191"/>
-      <c r="E30" s="192"/>
-      <c r="F30" s="192"/>
-      <c r="G30" s="192"/>
-      <c r="H30" s="192"/>
-      <c r="I30" s="192"/>
-      <c r="J30" s="192"/>
+      <c r="C30" s="192"/>
+      <c r="D30" s="192"/>
+      <c r="E30" s="191"/>
+      <c r="F30" s="191"/>
+      <c r="G30" s="191"/>
+      <c r="H30" s="191"/>
+      <c r="I30" s="191"/>
+      <c r="J30" s="191"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="191"/>
-      <c r="C31" s="191"/>
-      <c r="D31" s="191"/>
-      <c r="E31" s="192"/>
-      <c r="F31" s="192"/>
-      <c r="G31" s="192"/>
-      <c r="H31" s="192"/>
-      <c r="I31" s="192"/>
-      <c r="J31" s="192"/>
+      <c r="B31" s="192"/>
+      <c r="C31" s="192"/>
+      <c r="D31" s="192"/>
+      <c r="E31" s="191"/>
+      <c r="F31" s="191"/>
+      <c r="G31" s="191"/>
+      <c r="H31" s="191"/>
+      <c r="I31" s="191"/>
+      <c r="J31" s="191"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -29174,7 +29174,7 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:B39"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -30672,7 +30672,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31187,7 +31187,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31273,17 +31273,17 @@
       <c r="D5" s="116">
         <v>1</v>
       </c>
-      <c r="F5" s="191" t="s">
+      <c r="F5" s="192" t="s">
         <v>1856</v>
       </c>
-      <c r="G5" s="191"/>
-      <c r="H5" s="191"/>
-      <c r="I5" s="191"/>
-      <c r="J5" s="191"/>
-      <c r="K5" s="191"/>
-      <c r="L5" s="191"/>
-      <c r="M5" s="191"/>
-      <c r="N5" s="191"/>
+      <c r="G5" s="192"/>
+      <c r="H5" s="192"/>
+      <c r="I5" s="192"/>
+      <c r="J5" s="192"/>
+      <c r="K5" s="192"/>
+      <c r="L5" s="192"/>
+      <c r="M5" s="192"/>
+      <c r="N5" s="192"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="116" t="s">
@@ -31298,15 +31298,15 @@
       <c r="D6" s="116">
         <v>1</v>
       </c>
-      <c r="F6" s="191"/>
-      <c r="G6" s="191"/>
-      <c r="H6" s="191"/>
-      <c r="I6" s="191"/>
-      <c r="J6" s="191"/>
-      <c r="K6" s="191"/>
-      <c r="L6" s="191"/>
-      <c r="M6" s="191"/>
-      <c r="N6" s="191"/>
+      <c r="F6" s="192"/>
+      <c r="G6" s="192"/>
+      <c r="H6" s="192"/>
+      <c r="I6" s="192"/>
+      <c r="J6" s="192"/>
+      <c r="K6" s="192"/>
+      <c r="L6" s="192"/>
+      <c r="M6" s="192"/>
+      <c r="N6" s="192"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>